<commit_message>
added a few dimension dictionaries
</commit_message>
<xml_diff>
--- a/Dictionary.xlsx
+++ b/Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\UPorto\MEIC\2ºAno\AID\AID-PROJ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dluis\Documents\Docs\Universidade\M 2 ano\AID\AID-PROJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E568D3DD-8457-4813-88F1-CC62559FC19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32E68A1-D430-434C-9D48-B86F026B3521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F98E924E-5EF0-45E0-BA33-9E7480F762B6}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="12777" windowHeight="13536" xr2:uid="{F98E924E-5EF0-45E0-BA33-9E7480F762B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Dimension" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="145">
   <si>
     <t>Description</t>
   </si>
@@ -119,6 +119,360 @@
   </si>
   <si>
     <t>Measures</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>A reviewer who did at least one review</t>
+  </si>
+  <si>
+    <t>Type 1</t>
+  </si>
+  <si>
+    <t>reviewer_id</t>
+  </si>
+  <si>
+    <t>reviewer_name</t>
+  </si>
+  <si>
+    <t>Reviewer identifier</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Reviewer name</t>
+  </si>
+  <si>
+    <t>Varchar</t>
+  </si>
+  <si>
+    <t>A specific date</t>
+  </si>
+  <si>
+    <t>date_id</t>
+  </si>
+  <si>
+    <t>SQL_date</t>
+  </si>
+  <si>
+    <t>Date identifier</t>
+  </si>
+  <si>
+    <t>Full date</t>
+  </si>
+  <si>
+    <t>day_id</t>
+  </si>
+  <si>
+    <t>day_number</t>
+  </si>
+  <si>
+    <t>month_id</t>
+  </si>
+  <si>
+    <t>month_name</t>
+  </si>
+  <si>
+    <t>month_number</t>
+  </si>
+  <si>
+    <t>year_id</t>
+  </si>
+  <si>
+    <t>year_number</t>
+  </si>
+  <si>
+    <t>Day identifier</t>
+  </si>
+  <si>
+    <t>Month identifier</t>
+  </si>
+  <si>
+    <t>Year identifier</t>
+  </si>
+  <si>
+    <t>Day number</t>
+  </si>
+  <si>
+    <t>Month name</t>
+  </si>
+  <si>
+    <t>Month number</t>
+  </si>
+  <si>
+    <t>Year number</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Listing Score</t>
+  </si>
+  <si>
+    <t>listing_score</t>
+  </si>
+  <si>
+    <t>Listing Score identifier</t>
+  </si>
+  <si>
+    <t>Date &lt; Day &lt; Month &lt; Year</t>
+  </si>
+  <si>
+    <t>review_scores_rating</t>
+  </si>
+  <si>
+    <t>review_scores_accuracy</t>
+  </si>
+  <si>
+    <t>review_scores_cleanliness</t>
+  </si>
+  <si>
+    <t>review_scores_checkin</t>
+  </si>
+  <si>
+    <t>review_scores_communication</t>
+  </si>
+  <si>
+    <t>review_scores_location</t>
+  </si>
+  <si>
+    <t>review_scores_value</t>
+  </si>
+  <si>
+    <t>reviews_per_month</t>
+  </si>
+  <si>
+    <t>Overall listing rating</t>
+  </si>
+  <si>
+    <t>How accurate the listing is</t>
+  </si>
+  <si>
+    <t>How cleaned is the property the listing pertains to</t>
+  </si>
+  <si>
+    <t>How good was the check-in</t>
+  </si>
+  <si>
+    <t>How good was the communication</t>
+  </si>
+  <si>
+    <t>How good was the location</t>
+  </si>
+  <si>
+    <t>How many reviews per month</t>
+  </si>
+  <si>
+    <t>How good it is in comparison to its price</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>The score people leave for the listing</t>
+  </si>
+  <si>
+    <t>The specifics of the property listed</t>
+  </si>
+  <si>
+    <t>property_id</t>
+  </si>
+  <si>
+    <t>accomodates</t>
+  </si>
+  <si>
+    <t>bedrooms</t>
+  </si>
+  <si>
+    <t>beds</t>
+  </si>
+  <si>
+    <t>amenities</t>
+  </si>
+  <si>
+    <t>square_feet</t>
+  </si>
+  <si>
+    <t>room_type_id</t>
+  </si>
+  <si>
+    <t>room_type</t>
+  </si>
+  <si>
+    <t>property_type_id</t>
+  </si>
+  <si>
+    <t>preperty_type</t>
+  </si>
+  <si>
+    <t>bathroom_type_id</t>
+  </si>
+  <si>
+    <t>bathroom_type</t>
+  </si>
+  <si>
+    <t>Property Identifier</t>
+  </si>
+  <si>
+    <t>How many people the property can have</t>
+  </si>
+  <si>
+    <t>The amount of bedrooms</t>
+  </si>
+  <si>
+    <t>The amount of beds</t>
+  </si>
+  <si>
+    <t>Which amenities the property provides</t>
+  </si>
+  <si>
+    <t>The property's square footage</t>
+  </si>
+  <si>
+    <t>Room type identifier</t>
+  </si>
+  <si>
+    <t>Room type</t>
+  </si>
+  <si>
+    <t>Property type identifier</t>
+  </si>
+  <si>
+    <t>Property type</t>
+  </si>
+  <si>
+    <t>Bathroom type identifier</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Bathroom</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Property &gt; Type; Property &gt; Room; Property &gt; Bathroom;</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>The host of a listing</t>
+  </si>
+  <si>
+    <t>host_id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>host_url</t>
+  </si>
+  <si>
+    <t>host_listing_count</t>
+  </si>
+  <si>
+    <t>host_total_listing_count</t>
+  </si>
+  <si>
+    <t>is_superhost</t>
+  </si>
+  <si>
+    <t>has_profile_pic</t>
+  </si>
+  <si>
+    <t>has_identity_verified</t>
+  </si>
+  <si>
+    <t>host_response_id</t>
+  </si>
+  <si>
+    <t>host_response_time</t>
+  </si>
+  <si>
+    <t>host_response_rate</t>
+  </si>
+  <si>
+    <t>host_acceptance_rate</t>
+  </si>
+  <si>
+    <t>host_verifications_id</t>
+  </si>
+  <si>
+    <t>Host identifier</t>
+  </si>
+  <si>
+    <t>Host name</t>
+  </si>
+  <si>
+    <t>Host description</t>
+  </si>
+  <si>
+    <t>Host page</t>
+  </si>
+  <si>
+    <t>The total number of listings the host has</t>
+  </si>
+  <si>
+    <t>The number of listing this is</t>
+  </si>
+  <si>
+    <t>Is the host a super host?</t>
+  </si>
+  <si>
+    <t>Does the host have a profile pic?</t>
+  </si>
+  <si>
+    <t>Does the host has its identity verified?</t>
+  </si>
+  <si>
+    <t>Host response identifier</t>
+  </si>
+  <si>
+    <t>Host response time</t>
+  </si>
+  <si>
+    <t>Host response rate</t>
+  </si>
+  <si>
+    <t>host_verifications</t>
+  </si>
+  <si>
+    <t>Host verifications identifier</t>
+  </si>
+  <si>
+    <t>The rate at which the host accepts booking requests</t>
+  </si>
+  <si>
+    <t>By which means the host accepts verifications</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Verifications</t>
+  </si>
+  <si>
+    <t>Boolean</t>
   </si>
 </sst>
 </file>
@@ -126,7 +480,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -181,7 +535,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -402,14 +756,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -420,9 +821,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -432,18 +830,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -451,15 +837,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -474,16 +851,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,102 +1187,1296 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01131C1E-E33D-4716-994E-D6710E865E13}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="C53" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="44.44140625" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="51.21875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="24"/>
-      <c r="B2" s="28" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="30">
+        <v>1</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="31">
+        <v>45253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
+      <c r="B3" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D4" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B5" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+    </row>
+    <row r="6" spans="1:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B6" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="32">
+        <v>50</v>
+      </c>
+      <c r="H6" s="32"/>
+    </row>
+    <row r="7" spans="1:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B9" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E9" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F9" s="30">
         <v>1</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G9" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="26">
-        <v>45251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="28" t="s">
+      <c r="H9" s="31">
+        <v>45253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B10" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-    </row>
-    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="24"/>
-      <c r="B4" s="28" t="s">
+      <c r="F10" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+    </row>
+    <row r="11" spans="1:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B11" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C11" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D11" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F11" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G11" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H11" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="24"/>
+    <row r="12" spans="1:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B12" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+    </row>
+    <row r="13" spans="1:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B13" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+    </row>
+    <row r="14" spans="1:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B14" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+    </row>
+    <row r="15" spans="1:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B15" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="32">
+        <v>1</v>
+      </c>
+      <c r="H15" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B16" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+    </row>
+    <row r="17" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B17" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="32">
+        <v>50</v>
+      </c>
+      <c r="H17" s="32"/>
+    </row>
+    <row r="18" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B18" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="32">
+        <v>1</v>
+      </c>
+      <c r="H18" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B19" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+    </row>
+    <row r="20" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B20" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="32">
+        <v>1</v>
+      </c>
+      <c r="H20" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B23" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="30">
+        <v>1</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="31">
+        <v>45253</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B24" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+    </row>
+    <row r="25" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B25" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B26" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+    </row>
+    <row r="27" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B27" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="32">
+        <v>1</v>
+      </c>
+      <c r="H27" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B28" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="32">
+        <v>1</v>
+      </c>
+      <c r="H28" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B29" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" s="32">
+        <v>1</v>
+      </c>
+      <c r="H29" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B30" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="32">
+        <v>1</v>
+      </c>
+      <c r="H30" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B31" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="32">
+        <v>1</v>
+      </c>
+      <c r="H31" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B32" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G32" s="32">
+        <v>1</v>
+      </c>
+      <c r="H32" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B33" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G33" s="32">
+        <v>1</v>
+      </c>
+      <c r="H33" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B34" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G34" s="32">
+        <v>1</v>
+      </c>
+      <c r="H34" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B37" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" s="30">
+        <v>1</v>
+      </c>
+      <c r="G37" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H37" s="31">
+        <v>45253</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B38" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+    </row>
+    <row r="39" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B39" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B40" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+    </row>
+    <row r="41" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B41" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+    </row>
+    <row r="42" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B42" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+    </row>
+    <row r="43" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B43" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+    </row>
+    <row r="44" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B44" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+    </row>
+    <row r="45" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B45" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+    </row>
+    <row r="46" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B46" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+    </row>
+    <row r="47" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B47" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D47" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G47" s="32">
+        <v>50</v>
+      </c>
+      <c r="H47" s="32"/>
+    </row>
+    <row r="48" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B48" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+    </row>
+    <row r="49" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B49" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C49" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D49" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G49" s="32">
+        <v>100</v>
+      </c>
+      <c r="H49" s="32"/>
+    </row>
+    <row r="50" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B50" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="E50" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+    </row>
+    <row r="51" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B51" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="34"/>
+      <c r="F51" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="G51" s="34">
+        <v>50</v>
+      </c>
+      <c r="H51" s="32"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B52" s="39"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="38"/>
+    </row>
+    <row r="54" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B54" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" s="30">
+        <v>1</v>
+      </c>
+      <c r="G54" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H54" s="31">
+        <v>45253</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B55" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55" s="33"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="33"/>
+    </row>
+    <row r="56" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B56" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H56" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B57" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D57" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E57" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+    </row>
+    <row r="58" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B58" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E58" s="32"/>
+      <c r="F58" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G58" s="32">
+        <v>50</v>
+      </c>
+      <c r="H58" s="32"/>
+    </row>
+    <row r="59" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B59" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E59" s="32"/>
+      <c r="F59" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G59" s="32">
+        <v>250</v>
+      </c>
+      <c r="H59" s="32"/>
+    </row>
+    <row r="60" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B60" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G60" s="32">
+        <v>50</v>
+      </c>
+      <c r="H60" s="32"/>
+    </row>
+    <row r="61" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B61" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="D61" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E61" s="32"/>
+      <c r="F61" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G61" s="32">
+        <v>1</v>
+      </c>
+      <c r="H61" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B62" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="D62" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E62" s="32"/>
+      <c r="F62" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G62" s="32">
+        <v>1</v>
+      </c>
+      <c r="H62" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B63" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="D63" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+    </row>
+    <row r="64" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B64" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="C64" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="D64" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G64" s="32"/>
+      <c r="H64" s="32"/>
+    </row>
+    <row r="65" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B65" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C65" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="D65" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E65" s="32"/>
+      <c r="F65" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G65" s="32"/>
+      <c r="H65" s="32"/>
+    </row>
+    <row r="66" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B66" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="C66" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="D66" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="E66" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G66" s="32"/>
+      <c r="H66" s="32"/>
+    </row>
+    <row r="67" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B67" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="D67" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="E67" s="32"/>
+      <c r="F67" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G67" s="32">
+        <v>50</v>
+      </c>
+      <c r="H67" s="32"/>
+    </row>
+    <row r="68" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B68" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="D68" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="E68" s="32"/>
+      <c r="F68" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G68" s="32">
+        <v>1</v>
+      </c>
+      <c r="H68" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B69" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="D69" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="E69" s="32"/>
+      <c r="F69" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G69" s="32">
+        <v>1</v>
+      </c>
+      <c r="H69" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B70" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C70" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="D70" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="E70" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G70" s="32"/>
+      <c r="H70" s="32"/>
+    </row>
+    <row r="71" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="B71" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="C71" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D71" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="E71" s="32"/>
+      <c r="F71" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="G71" s="32"/>
+      <c r="H71" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F55:H55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -901,11 +2484,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92297134-47BA-4AE1-96C7-D70C00EEB25B}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.5546875" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
@@ -914,241 +2497,241 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="24"/>
-      <c r="B2" s="28" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="28" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="6">
         <v>1</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="26">
+      <c r="G2" s="7">
         <v>45251</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="24"/>
-      <c r="B3" s="28" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="24"/>
-      <c r="B4" s="28" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="24"/>
-      <c r="B7" s="28" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-    </row>
-    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-    </row>
-    <row r="17" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" ht="18.350000000000001" x14ac:dyDescent="0.35">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1167,29 +2750,29 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:17" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15"/>
-      <c r="N3" s="16" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+      <c r="N3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="18"/>
-    </row>
-    <row r="4" spans="2:17" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="28"/>
+    </row>
+    <row r="4" spans="2:17" ht="34.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -1201,58 +2784,58 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="12"/>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="19"/>
-    </row>
-    <row r="5" spans="2:17" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P4" s="14"/>
+      <c r="Q4" s="22"/>
+    </row>
+    <row r="5" spans="2:17" ht="34.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="4"/>
-      <c r="N5" s="23" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
+      <c r="N5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="20" t="s">
+      <c r="O5" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="22"/>
-    </row>
-    <row r="6" spans="2:17" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="5" t="s">
+      <c r="P5" s="24"/>
+      <c r="Q5" s="25"/>
+    </row>
+    <row r="6" spans="2:17" ht="34.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="8"/>
-      <c r="N6" s="23" t="s">
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
+      <c r="N6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="20" t="s">
+      <c r="O6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="22"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Update sizes in dictionaries
</commit_message>
<xml_diff>
--- a/Dictionary.xlsx
+++ b/Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dluis\Documents\Docs\Universidade\M 2 ano\AID\AID-PROJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07063655-9006-43E7-8B02-4513AACC160A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C3B11A-92DD-486A-9D27-42432607C6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" xr2:uid="{F98E924E-5EF0-45E0-BA33-9E7480F762B6}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" activeTab="1" xr2:uid="{F98E924E-5EF0-45E0-BA33-9E7480F762B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Dimension" sheetId="1" r:id="rId1"/>
@@ -942,7 +942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -963,16 +963,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1032,17 +1042,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1359,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01131C1E-E33D-4716-994E-D6710E865E13}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView topLeftCell="A9" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1423,11 +1422,11 @@
       <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
@@ -1545,11 +1544,11 @@
       <c r="E10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
@@ -1785,11 +1784,11 @@
       <c r="E24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
@@ -1928,7 +1927,7 @@
         <v>35</v>
       </c>
       <c r="G31" s="9">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H31" s="9"/>
     </row>
@@ -1947,7 +1946,7 @@
         <v>35</v>
       </c>
       <c r="G32" s="9">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H32" s="9"/>
     </row>
@@ -1965,8 +1964,8 @@
       <c r="F33" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="10">
-        <v>100</v>
+      <c r="G33" s="9">
+        <v>50</v>
       </c>
       <c r="H33" s="9"/>
     </row>
@@ -2014,11 +2013,11 @@
       <c r="E37" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F37" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
     </row>
     <row r="38" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="B38" s="6" t="s">
@@ -2096,7 +2095,7 @@
         <v>35</v>
       </c>
       <c r="G41" s="9">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="H41" s="9"/>
     </row>
@@ -2115,7 +2114,7 @@
         <v>35</v>
       </c>
       <c r="G42" s="9">
-        <v>50</v>
+        <v>255</v>
       </c>
       <c r="H42" s="9"/>
     </row>
@@ -2343,11 +2342,11 @@
       <c r="E56" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F56" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
     </row>
     <row r="57" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="B57" s="6" t="s">
@@ -2611,8 +2610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92297134-47BA-4AE1-96C7-D70C00EEB25B}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -2666,13 +2665,13 @@
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -2680,14 +2679,14 @@
     </row>
     <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -2763,14 +2762,14 @@
     </row>
     <row r="9" spans="1:11" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -2866,13 +2865,13 @@
       <c r="B15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -2880,14 +2879,14 @@
     </row>
     <row r="16" spans="1:11" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -2959,14 +2958,14 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:11" ht="18.350000000000001" x14ac:dyDescent="0.35">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
     </row>
     <row r="23" spans="1:11" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="B23" s="9" t="s">
@@ -2984,13 +2983,13 @@
       <c r="B24" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="37"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
     </row>
     <row r="25" spans="1:11" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="B25" s="9" t="s">
@@ -3004,7 +3003,7 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="B26" s="9" t="s">
         <v>61</v>
       </c>
@@ -3092,56 +3091,56 @@
       <c r="B33" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C33" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="38"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="12"/>
     </row>
     <row r="34" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="B34" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="38"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="12"/>
     </row>
     <row r="35" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="B35" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="38"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="12"/>
     </row>
     <row r="36" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="B36" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="38"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="12"/>
     </row>
     <row r="37" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="9" t="s">
         <v>179</v>
       </c>
       <c r="C37" s="14" t="s">
@@ -3176,23 +3175,23 @@
       <c r="B41" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
     </row>
     <row r="42" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="B43" s="9" t="s">
@@ -3207,14 +3206,14 @@
       <c r="G43" s="14"/>
     </row>
     <row r="44" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
     </row>
     <row r="45" spans="2:8" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="B45" s="9" t="s">
@@ -3266,6 +3265,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="C48:G48"/>
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="C35:G35"/>
@@ -3282,30 +3305,6 @@
     <mergeCell ref="C28:G28"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="C43:G43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3324,88 +3323,88 @@
   <sheetData>
     <row r="2" spans="2:17" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27"/>
-      <c r="N3" s="32" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="31"/>
+      <c r="N3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="34"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="38"/>
     </row>
     <row r="4" spans="2:17" ht="34.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="18"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22"/>
       <c r="N4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="O4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="28"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="32"/>
     </row>
     <row r="5" spans="2:17" ht="34.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25"/>
       <c r="N5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="29" t="s">
+      <c r="O5" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="31"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="35"/>
     </row>
     <row r="6" spans="2:17" ht="34.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
       <c r="N6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="29" t="s">
+      <c r="O6" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="31"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>